<commit_message>
added mummiochog correlation fxns
</commit_message>
<xml_diff>
--- a/Outputs/Annotation/QC.xlsx
+++ b/Outputs/Annotation/QC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/DTC-metabolomics-2026/Outputs/Annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC92778-D5EF-3645-984E-3E657B68E644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786E247A-43F4-D345-9CD1-60CC69B9EC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QC" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">QC!$A$1:$Y$291</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -5287,7 +5286,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:E5"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated correlation matrix to include citrulline
</commit_message>
<xml_diff>
--- a/Outputs/Annotation/QC.xlsx
+++ b/Outputs/Annotation/QC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/DTC-metabolomics-2026/Outputs/Annotation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdp2019/Desktop/DTC-metabolomics-2026/Outputs/Annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA4C92B-048F-F245-B6F4-271E97636794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D5235F-56F5-BB4A-8A06-1F6857840FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-11640" windowWidth="21600" windowHeight="36920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QC" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4015" uniqueCount="1622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4016" uniqueCount="1622">
   <si>
     <t>Identified Name</t>
   </si>
@@ -5334,9 +5334,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624A435F-8BE2-214B-91C7-3973CD222FA7}">
   <dimension ref="A1:Z133"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
+      <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6856,7 +6856,9 @@
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
+      <c r="L21" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4" t="s">
         <v>7</v>
@@ -14972,8 +14974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0EDF12F-ACFA-854C-BF7A-D84A1BAF082E}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>